<commit_message>
update rooms in SWFIS and U2
</commit_message>
<xml_diff>
--- a/timetable_scheduler/data_structures/data/schedule.xlsx
+++ b/timetable_scheduler/data_structures/data/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumenty\studia\Semestr 5\Badania operacyjne 2\timetable-scheduler\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumenty\studia\Semestr 5\Badania operacyjne 2\timetable-scheduler\timetable_scheduler\data_structures\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B5DAA42-5904-402E-A4B0-E4A351BE60DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB91DA2-CBAE-4AF2-A929-46D393C1D9DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -103,9 +103,6 @@
     <t>Wychowanie fizyczne 1</t>
   </si>
   <si>
-    <t>SWFIS</t>
-  </si>
-  <si>
     <t>Fizyka 2</t>
   </si>
   <si>
@@ -139,9 +136,6 @@
     <t>Inzynieria procesow produkcyjnych</t>
   </si>
   <si>
-    <t>U2</t>
-  </si>
-  <si>
     <t>Teoria obwodow</t>
   </si>
   <si>
@@ -347,12 +341,18 @@
   </si>
   <si>
     <t>Przedmiot humanistyczny</t>
+  </si>
+  <si>
+    <t>SWFIS-1</t>
+  </si>
+  <si>
+    <t>U2-1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1204,11 +1204,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1444,7 +1444,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1452,7 +1452,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -1473,12 +1473,12 @@
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -1504,7 +1504,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -1522,7 +1522,7 @@
         <v>15</v>
       </c>
       <c r="G12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -1530,7 +1530,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -1556,7 +1556,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -1582,7 +1582,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -1608,7 +1608,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -1629,12 +1629,12 @@
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -1649,7 +1649,7 @@
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>39</v>
+        <v>108</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -1660,7 +1660,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -1678,7 +1678,7 @@
         <v>12</v>
       </c>
       <c r="G18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -1686,7 +1686,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -1704,7 +1704,7 @@
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -1712,7 +1712,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -1733,12 +1733,12 @@
         <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B21">
         <v>3</v>
@@ -1753,7 +1753,7 @@
         <v>28</v>
       </c>
       <c r="F21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -1764,7 +1764,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B22">
         <v>3</v>
@@ -1779,7 +1779,7 @@
         <v>28</v>
       </c>
       <c r="F22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -1790,7 +1790,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B23">
         <v>3</v>
@@ -1805,18 +1805,18 @@
         <v>28</v>
       </c>
       <c r="F23" t="s">
-        <v>39</v>
+        <v>108</v>
       </c>
       <c r="G23">
         <v>0</v>
       </c>
       <c r="H23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -1837,12 +1837,12 @@
         <v>0</v>
       </c>
       <c r="H24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B25">
         <v>3</v>
@@ -1868,7 +1868,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B26">
         <v>3</v>
@@ -1883,18 +1883,18 @@
         <v>14</v>
       </c>
       <c r="F26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G26">
         <v>0</v>
       </c>
       <c r="H26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B27">
         <v>3</v>
@@ -1909,18 +1909,18 @@
         <v>28</v>
       </c>
       <c r="F27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G27">
         <v>0</v>
       </c>
       <c r="H27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B28">
         <v>3</v>
@@ -1938,7 +1938,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="H28">
         <v>0</v>
@@ -1946,7 +1946,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B29">
         <v>3</v>
@@ -1967,12 +1967,12 @@
         <v>0</v>
       </c>
       <c r="H29" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B30">
         <v>4</v>
@@ -1998,7 +1998,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B31">
         <v>4</v>
@@ -2019,12 +2019,12 @@
         <v>0</v>
       </c>
       <c r="H31" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B32">
         <v>4</v>
@@ -2045,12 +2045,12 @@
         <v>0</v>
       </c>
       <c r="H32" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B33">
         <v>4</v>
@@ -2071,12 +2071,12 @@
         <v>0</v>
       </c>
       <c r="H33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B34">
         <v>4</v>
@@ -2091,18 +2091,18 @@
         <v>28</v>
       </c>
       <c r="F34" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G34">
         <v>0</v>
       </c>
       <c r="H34" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B35">
         <v>4</v>
@@ -2123,12 +2123,12 @@
         <v>0</v>
       </c>
       <c r="H35" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B36">
         <v>4</v>
@@ -2143,18 +2143,18 @@
         <v>28</v>
       </c>
       <c r="F36" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G36">
         <v>0</v>
       </c>
       <c r="H36" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B37">
         <v>4</v>
@@ -2180,7 +2180,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B38">
         <v>4</v>
@@ -2201,12 +2201,12 @@
         <v>0</v>
       </c>
       <c r="H38" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -2227,12 +2227,12 @@
         <v>0</v>
       </c>
       <c r="H39" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B40">
         <v>5</v>
@@ -2253,12 +2253,12 @@
         <v>0</v>
       </c>
       <c r="H40" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B41">
         <v>5</v>
@@ -2279,12 +2279,12 @@
         <v>0</v>
       </c>
       <c r="H41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B42">
         <v>5</v>
@@ -2305,12 +2305,12 @@
         <v>10</v>
       </c>
       <c r="H42" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B43">
         <v>5</v>
@@ -2328,7 +2328,7 @@
         <v>15</v>
       </c>
       <c r="G43" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H43">
         <v>0</v>
@@ -2336,7 +2336,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B44">
         <v>5</v>
@@ -2351,18 +2351,18 @@
         <v>28</v>
       </c>
       <c r="F44" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G44">
         <v>0</v>
       </c>
       <c r="H44" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B45">
         <v>5</v>
@@ -2377,18 +2377,18 @@
         <v>28</v>
       </c>
       <c r="F45" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G45">
         <v>0</v>
       </c>
       <c r="H45" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B46">
         <v>5</v>
@@ -2414,7 +2414,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B47">
         <v>5</v>
@@ -2429,18 +2429,18 @@
         <v>28</v>
       </c>
       <c r="F47" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G47">
         <v>0</v>
       </c>
       <c r="H47" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B48">
         <v>5</v>
@@ -2455,18 +2455,18 @@
         <v>28</v>
       </c>
       <c r="F48" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G48">
         <v>0</v>
       </c>
       <c r="H48" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B49">
         <v>6</v>
@@ -2481,7 +2481,7 @@
         <v>0</v>
       </c>
       <c r="F49" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -2492,7 +2492,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B50">
         <v>6</v>
@@ -2513,12 +2513,12 @@
         <v>0</v>
       </c>
       <c r="H50" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B51">
         <v>6</v>
@@ -2539,12 +2539,12 @@
         <v>0</v>
       </c>
       <c r="H51" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B52">
         <v>6</v>
@@ -2565,12 +2565,12 @@
         <v>0</v>
       </c>
       <c r="H52" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B53">
         <v>6</v>
@@ -2591,12 +2591,12 @@
         <v>0</v>
       </c>
       <c r="H53" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B54">
         <v>6</v>
@@ -2617,12 +2617,12 @@
         <v>0</v>
       </c>
       <c r="H54" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B55">
         <v>6</v>
@@ -2637,7 +2637,7 @@
         <v>28</v>
       </c>
       <c r="F55" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G55">
         <v>0</v>
@@ -2648,7 +2648,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B56">
         <v>6</v>
@@ -2669,12 +2669,12 @@
         <v>0</v>
       </c>
       <c r="H56" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B57">
         <v>6</v>
@@ -2689,7 +2689,7 @@
         <v>28</v>
       </c>
       <c r="F57" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G57">
         <v>0</v>
@@ -2700,7 +2700,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B58">
         <v>7</v>
@@ -2721,12 +2721,12 @@
         <v>0</v>
       </c>
       <c r="H58" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B59">
         <v>7</v>
@@ -2752,7 +2752,7 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B60">
         <v>7</v>
@@ -2773,12 +2773,12 @@
         <v>0</v>
       </c>
       <c r="H60" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B61">
         <v>7</v>
@@ -2799,12 +2799,12 @@
         <v>0</v>
       </c>
       <c r="H61" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B62">
         <v>7</v>
@@ -2819,18 +2819,18 @@
         <v>14</v>
       </c>
       <c r="F62" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G62">
         <v>0</v>
       </c>
       <c r="H62" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B63">
         <v>7</v>
@@ -2851,12 +2851,12 @@
         <v>0</v>
       </c>
       <c r="H63" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B64">
         <v>7</v>
@@ -2882,7 +2882,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B65">
         <v>7</v>
@@ -2897,7 +2897,7 @@
         <v>0</v>
       </c>
       <c r="F65" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G65">
         <v>0</v>
@@ -2908,7 +2908,7 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B66">
         <v>7</v>
@@ -2923,7 +2923,7 @@
         <v>0</v>
       </c>
       <c r="F66" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G66">
         <v>0</v>
@@ -2934,7 +2934,7 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B67">
         <v>7</v>
@@ -2949,7 +2949,7 @@
         <v>0</v>
       </c>
       <c r="F67" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G67">
         <v>0</v>

</xml_diff>